<commit_message>
Update Revision History - Figma.xlsx
Update file. Add sign for use case diagram
</commit_message>
<xml_diff>
--- a/Documenti di Progetto/Revision History - Figma.xlsx
+++ b/Documenti di Progetto/Revision History - Figma.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raffaella/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\salva\GitHub\WoodLot\Documenti di Progetto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6AC4EB2-A5DA-214C-80ED-068065B6D375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B9EBCC0-B270-4E22-883E-F94E51AD2F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15840" xr2:uid="{4A92E1C4-0C03-B648-8F37-4C727B03EE17}"/>
+    <workbookView xWindow="3450" yWindow="2550" windowWidth="21600" windowHeight="11295" xr2:uid="{4A92E1C4-0C03-B648-8F37-4C727B03EE17}"/>
   </bookViews>
   <sheets>
     <sheet name="Use Case Diagram" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>DATA</t>
   </si>
@@ -60,6 +60,15 @@
   </si>
   <si>
     <t>REVISON HISTORY - USE CASE DIAGRAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use Case Diagram Ospite </t>
+  </si>
+  <si>
+    <t>SDS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use Case Diagram Utente </t>
   </si>
 </sst>
 </file>
@@ -103,7 +112,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -120,14 +129,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -139,6 +148,9 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -154,7 +166,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BFD3B3F1-39AF-574B-B4E2-6DD2F98814AC}" name="Tabella1" displayName="Tabella1" ref="B2:E23" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BFD3B3F1-39AF-574B-B4E2-6DD2F98814AC}" name="Tabella1" displayName="Tabella1" ref="B2:E23" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="B2:E23" xr:uid="{BFD3B3F1-39AF-574B-B4E2-6DD2F98814AC}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -162,10 +174,10 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{D2472224-3F02-2744-8657-6A872C869000}" name="DATA" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{7FA9BCB9-E897-B440-9BF5-675437705F38}" name="VERSIONE" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{287F26B4-1CCD-AC44-AD6B-D76F16EAB32B}" name="DESCRIZIONE" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{8213545A-71F5-B24E-B9A1-3418391DCE22}" name="AUTORE" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{D2472224-3F02-2744-8657-6A872C869000}" name="DATA" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{7FA9BCB9-E897-B440-9BF5-675437705F38}" name="VERSIONE" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{287F26B4-1CCD-AC44-AD6B-D76F16EAB32B}" name="DESCRIZIONE" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{8213545A-71F5-B24E-B9A1-3418391DCE22}" name="AUTORE" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -471,19 +483,19 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" style="3" customWidth="1"/>
-    <col min="2" max="2" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B1" s="5" t="s">
         <v>7</v>
       </c>
@@ -491,7 +503,7 @@
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -505,7 +517,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="2">
         <v>44860</v>
       </c>
@@ -519,121 +531,137 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="3"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="3"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="6">
+        <v>44861</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="6">
+        <v>44861</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" s="1"/>
       <c r="D6" s="4"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
       <c r="C7" s="1"/>
       <c r="D7" s="4"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="3"/>
       <c r="C8" s="1"/>
       <c r="D8" s="4"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="3"/>
       <c r="C9" s="1"/>
       <c r="D9" s="4"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
       <c r="C10" s="1"/>
       <c r="D10" s="4"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="3"/>
       <c r="C11" s="1"/>
       <c r="D11" s="4"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="3"/>
       <c r="C12" s="1"/>
       <c r="D12" s="4"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="3"/>
       <c r="C13" s="1"/>
       <c r="D13" s="4"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
       <c r="C14" s="1"/>
       <c r="D14" s="4"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
       <c r="C15" s="1"/>
       <c r="D15" s="4"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
       <c r="C16" s="1"/>
       <c r="D16" s="4"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3"/>
       <c r="C17" s="1"/>
       <c r="D17" s="4"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
       <c r="C18" s="1"/>
       <c r="D18" s="4"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
       <c r="C19" s="1"/>
       <c r="D19" s="4"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
       <c r="C20" s="1"/>
       <c r="D20" s="4"/>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3"/>
       <c r="C21" s="1"/>
       <c r="D21" s="4"/>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3"/>
       <c r="C22" s="1"/>
       <c r="D22" s="4"/>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3"/>
       <c r="C23" s="1"/>
       <c r="D23" s="4"/>

</xml_diff>

<commit_message>
Revision Hisdtory - Figma
Aggiunte di AT e RS, modifica errori di SDS
</commit_message>
<xml_diff>
--- a/Documenti di Progetto/Revision History - Figma.xlsx
+++ b/Documenti di Progetto/Revision History - Figma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raffaella/Documents/WoodLot/Documenti di Progetto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB480D5-3CAE-F94B-965D-56F9144035D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B37AC483-71D8-1E4A-B267-7193C316C9EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3460" yWindow="2560" windowWidth="21600" windowHeight="11300" xr2:uid="{4A92E1C4-0C03-B648-8F37-4C727B03EE17}"/>
+    <workbookView xWindow="4960" yWindow="-15260" windowWidth="21600" windowHeight="11300" xr2:uid="{4A92E1C4-0C03-B648-8F37-4C727B03EE17}"/>
   </bookViews>
   <sheets>
     <sheet name="Use Case Diagram" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>DATA</t>
   </si>
@@ -62,13 +62,25 @@
     <t>REVISON HISTORY - USE CASE DIAGRAM</t>
   </si>
   <si>
-    <t xml:space="preserve">Use Case Diagram Ospite </t>
-  </si>
-  <si>
     <t>SDS</t>
   </si>
   <si>
-    <t xml:space="preserve">Use Case Diagram Utente </t>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aggiunta Use Case Diagram Ospite </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aggiunta Use Case Diagram Utente </t>
+  </si>
+  <si>
+    <t>Aggiunta Use Case Diagram Contadino</t>
+  </si>
+  <si>
+    <t>RS</t>
+  </si>
+  <si>
+    <t>Aggiunta Use Case Diagram Catalogo</t>
   </si>
 </sst>
 </file>
@@ -479,8 +491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9A7717B-E787-F440-A477-62CF32499A0B}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -532,70 +544,76 @@
       <c r="B4" s="2">
         <v>44861</v>
       </c>
-      <c r="C4" s="1">
-        <v>1</v>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="2">
         <v>44861</v>
       </c>
-      <c r="C5" s="1">
-        <v>1</v>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B6" s="2">
+        <v>44864</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="3"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="3"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="1"/>
+      <c r="B7" s="2">
+        <v>44864</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="3"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="4"/>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="3"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="4"/>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="3"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="4"/>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="3"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="4"/>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="3"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="4"/>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Archivio Agenda e Minute
Aggiunta Weekly Meeting 6
</commit_message>
<xml_diff>
--- a/Documenti di Progetto/Revision History - Figma.xlsx
+++ b/Documenti di Progetto/Revision History - Figma.xlsx
@@ -1,19 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\salva\GitHub\WoodLot\Documenti di Progetto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raffaella/Documents/WoodLot/Documenti di Progetto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D4970C-889E-4ECF-A307-8D11A1F1FC8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFE98416-9567-5249-8858-16E00F5AB5B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4A92E1C4-0C03-B648-8F37-4C727B03EE17}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" activeTab="3" xr2:uid="{4A92E1C4-0C03-B648-8F37-4C727B03EE17}"/>
   </bookViews>
   <sheets>
-    <sheet name="Use Case Diagram" sheetId="1" r:id="rId1"/>
+    <sheet name="Mock-up" sheetId="5" r:id="rId1"/>
+    <sheet name="Use Case Diagram" sheetId="1" r:id="rId2"/>
+    <sheet name="Statechart Diagram" sheetId="3" r:id="rId3"/>
+    <sheet name="Navigational Path" sheetId="7" r:id="rId4"/>
+    <sheet name="Class Diagram" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="26">
   <si>
     <t>DATA</t>
   </si>
@@ -102,6 +106,18 @@
   </si>
   <si>
     <t>Aggiunta StateChart</t>
+  </si>
+  <si>
+    <t>REVISON HISTORY - STATECHRT DIAGRAM</t>
+  </si>
+  <si>
+    <t>REVISON HISTORY - MOCK-UP</t>
+  </si>
+  <si>
+    <t>REVISON HISTORY - CLASS DIAGRAM</t>
+  </si>
+  <si>
+    <t>REVISON HISTORY - NAVIGATIONAL PATH</t>
   </si>
 </sst>
 </file>
@@ -166,7 +182,67 @@
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="25">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -196,7 +272,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BFD3B3F1-39AF-574B-B4E2-6DD2F98814AC}" name="Tabella1" displayName="Tabella1" ref="B2:E23" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{04D74344-D276-384C-86AC-E6FCBC66F272}" name="Tabella15" displayName="Tabella15" ref="B2:E23" totalsRowShown="0" headerRowDxfId="14">
   <autoFilter ref="B2:E23" xr:uid="{BFD3B3F1-39AF-574B-B4E2-6DD2F98814AC}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -204,10 +280,82 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{D2472224-3F02-2744-8657-6A872C869000}" name="DATA" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{7FA9BCB9-E897-B440-9BF5-675437705F38}" name="VERSIONE" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{287F26B4-1CCD-AC44-AD6B-D76F16EAB32B}" name="DESCRIZIONE" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{8213545A-71F5-B24E-B9A1-3418391DCE22}" name="AUTORE" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{9CE3F216-5F00-C949-B764-1C474BC4E6F7}" name="DATA" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{B65B1588-D391-084E-B362-96ACBB55D55F}" name="VERSIONE" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{5A35C614-6143-2E41-B770-E9159B831AC1}" name="DESCRIZIONE" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{9279B9EE-E335-9A4B-A08C-E21EB6909A98}" name="AUTORE" dataDxfId="10"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BFD3B3F1-39AF-574B-B4E2-6DD2F98814AC}" name="Tabella1" displayName="Tabella1" ref="B2:E23" totalsRowShown="0" headerRowDxfId="24">
+  <autoFilter ref="B2:E23" xr:uid="{BFD3B3F1-39AF-574B-B4E2-6DD2F98814AC}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{D2472224-3F02-2744-8657-6A872C869000}" name="DATA" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{7FA9BCB9-E897-B440-9BF5-675437705F38}" name="VERSIONE" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{287F26B4-1CCD-AC44-AD6B-D76F16EAB32B}" name="DESCRIZIONE" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{8213545A-71F5-B24E-B9A1-3418391DCE22}" name="AUTORE" dataDxfId="20"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8E559B2E-DA0D-F143-8EFE-D37F837E0651}" name="Tabella14" displayName="Tabella14" ref="B2:E23" totalsRowShown="0" headerRowDxfId="19">
+  <autoFilter ref="B2:E23" xr:uid="{BFD3B3F1-39AF-574B-B4E2-6DD2F98814AC}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{378C1216-916E-5544-9728-AA01BCB8B490}" name="DATA" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{C0CC21E6-1BDA-674A-BF46-2171B580AC90}" name="VERSIONE" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{120155EA-3E0E-6B4B-A0E1-2E2B0D2F3140}" name="DESCRIZIONE" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{93260112-5814-1241-B832-6563BE25C71F}" name="AUTORE" dataDxfId="15"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{54B71CEB-3BE9-2D43-9426-5BB1E770D4EF}" name="Tabella1467" displayName="Tabella1467" ref="B2:E23" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="B2:E23" xr:uid="{BFD3B3F1-39AF-574B-B4E2-6DD2F98814AC}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{EFC912E6-D157-384A-99D5-25B94006AD03}" name="DATA" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{047CD72C-0FBB-A641-99FF-B5F32B6A45C6}" name="VERSIONE" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{57F48B9D-75F1-C546-BE4B-0968141ED3E5}" name="DESCRIZIONE" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{9D7F8A0A-9573-854B-88DF-998DF658CB24}" name="AUTORE" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C631A97A-F7D8-594B-B7D2-25620C66AA81}" name="Tabella146" displayName="Tabella146" ref="B2:E23" totalsRowShown="0" headerRowDxfId="9">
+  <autoFilter ref="B2:E23" xr:uid="{BFD3B3F1-39AF-574B-B4E2-6DD2F98814AC}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{7C7AFF3E-F623-924D-A0B4-16386F27322B}" name="DATA" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{1C2CD86D-9E3B-5A4A-9634-44B2F9F64A34}" name="VERSIONE" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{6B5D89E2-E9F3-0348-AC4F-276719705EF0}" name="DESCRIZIONE" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{6F8E928E-C13E-3441-945B-4D39C4C14E21}" name="AUTORE" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -509,31 +657,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9A7717B-E787-F440-A477-62CF32499A0B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{256147BA-D926-674E-96C3-5C4EE21DE2A0}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B12"/>
+    <sheetView zoomScale="135" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B1" s="5" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -547,207 +695,881 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="2">
-        <v>44860</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="2">
-        <v>44861</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="2">
-        <v>44861</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="2">
-        <v>44864</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="2">
-        <v>44864</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="2">
-        <v>44865</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="2">
-        <v>44865</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="2">
-        <v>44865</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="2">
-        <v>44865</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="2">
-        <v>44871</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B3" s="2"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B4" s="2"/>
+      <c r="C4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B5" s="2"/>
+      <c r="C5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B6" s="2"/>
+      <c r="C6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B7" s="2"/>
+      <c r="C7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B8" s="2"/>
+      <c r="C8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="2"/>
+      <c r="C9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="2"/>
+      <c r="C10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="2"/>
+      <c r="C11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B12" s="2"/>
+      <c r="C12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B13" s="3"/>
       <c r="C13" s="1"/>
       <c r="D13" s="4"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B14" s="3"/>
       <c r="C14" s="1"/>
       <c r="D14" s="4"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B15" s="3"/>
       <c r="C15" s="1"/>
       <c r="D15" s="4"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B16" s="3"/>
       <c r="C16" s="1"/>
       <c r="D16" s="4"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" s="3"/>
       <c r="C17" s="1"/>
       <c r="D17" s="4"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" s="3"/>
       <c r="C18" s="1"/>
       <c r="D18" s="4"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" s="3"/>
       <c r="C19" s="1"/>
       <c r="D19" s="4"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" s="3"/>
       <c r="C20" s="1"/>
       <c r="D20" s="4"/>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" s="3"/>
       <c r="C21" s="1"/>
       <c r="D21" s="4"/>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B22" s="3"/>
       <c r="C22" s="1"/>
       <c r="D22" s="4"/>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B23" s="3"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9A7717B-E787-F440-A477-62CF32499A0B}">
+  <dimension ref="A1:E23"/>
+  <sheetViews>
+    <sheetView zoomScale="135" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:E23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17" style="3" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B3" s="2">
+        <v>44860</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B4" s="2">
+        <v>44861</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B5" s="2">
+        <v>44861</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B6" s="2">
+        <v>44864</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B7" s="2">
+        <v>44864</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B8" s="2">
+        <v>44865</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="2">
+        <v>44865</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="2">
+        <v>44865</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="2">
+        <v>44865</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B12" s="2">
+        <v>44871</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B13" s="3"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B14" s="3"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B15" s="3"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="3"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="3"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="3"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="3"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="3"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B21" s="3"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B22" s="3"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B23" s="3"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69F97323-D4EC-FD45-9D8F-7A5F3A227394}">
+  <dimension ref="A1:E23"/>
+  <sheetViews>
+    <sheetView zoomScale="135" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17" style="3" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B3" s="2">
+        <v>44871</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B4" s="2"/>
+      <c r="C4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B5" s="2"/>
+      <c r="C5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B6" s="2"/>
+      <c r="C6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B7" s="2"/>
+      <c r="C7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B8" s="2"/>
+      <c r="C8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="2"/>
+      <c r="C9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="2"/>
+      <c r="C10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="2"/>
+      <c r="C11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B12" s="2"/>
+      <c r="C12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B13" s="3"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B14" s="3"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B15" s="3"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="3"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="3"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="3"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="3"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="3"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B21" s="3"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B22" s="3"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B23" s="3"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AF668EB-F66C-0745-B382-56EACCF4771A}">
+  <dimension ref="A1:E23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17" style="3" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B3" s="2"/>
+      <c r="C3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B4" s="2"/>
+      <c r="C4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B5" s="2"/>
+      <c r="C5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B6" s="2"/>
+      <c r="C6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B7" s="2"/>
+      <c r="C7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B8" s="2"/>
+      <c r="C8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="2"/>
+      <c r="C9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="2"/>
+      <c r="C10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="2"/>
+      <c r="C11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B12" s="2"/>
+      <c r="C12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B13" s="3"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B14" s="3"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B15" s="3"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="3"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="3"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="3"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="3"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="3"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B21" s="3"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B22" s="3"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B23" s="3"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC713557-CF4C-3449-B7F2-607954CE9E41}">
+  <dimension ref="A1:E23"/>
+  <sheetViews>
+    <sheetView zoomScale="135" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17" style="3" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B3" s="2"/>
+      <c r="C3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B4" s="2"/>
+      <c r="C4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B5" s="2"/>
+      <c r="C5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B6" s="2"/>
+      <c r="C6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B7" s="2"/>
+      <c r="C7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B8" s="2"/>
+      <c r="C8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="2"/>
+      <c r="C9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="2"/>
+      <c r="C10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="2"/>
+      <c r="C11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B12" s="2"/>
+      <c r="C12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B13" s="3"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B14" s="3"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B15" s="3"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="3"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="3"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="3"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="3"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="3"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B21" s="3"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B22" s="3"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" s="3"/>
       <c r="C23" s="1"/>
       <c r="D23" s="4"/>

</xml_diff>

<commit_message>
Revision History - Figma
Sequence Diagram, Navigational Path, Class Diagram
</commit_message>
<xml_diff>
--- a/Documenti di Progetto/Revision History - Figma.xlsx
+++ b/Documenti di Progetto/Revision History - Figma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raffaella/Documents/WoodLot/Documenti di Progetto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F32131A-821A-3043-B17A-57DB634FEC3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE95B3AE-ED08-8443-A26D-B9FCAE2C6ABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="500" windowWidth="25380" windowHeight="15720" activeTab="1" xr2:uid="{4A92E1C4-0C03-B648-8F37-4C727B03EE17}"/>
+    <workbookView xWindow="3420" yWindow="500" windowWidth="25380" windowHeight="15720" activeTab="5" xr2:uid="{4A92E1C4-0C03-B648-8F37-4C727B03EE17}"/>
   </bookViews>
   <sheets>
     <sheet name="Sequence Diagram" sheetId="9" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="76">
   <si>
     <t>DATA</t>
   </si>
@@ -248,6 +248,27 @@
   </si>
   <si>
     <t>Creazione form TreeCode</t>
+  </si>
+  <si>
+    <t>Revisione SD - Logout</t>
+  </si>
+  <si>
+    <t>Revisione SD - Aggiungere Prodotto</t>
+  </si>
+  <si>
+    <t>Revisione SD - Modificare Quantità</t>
+  </si>
+  <si>
+    <t>Revisione SD - Eliminare Prodotto</t>
+  </si>
+  <si>
+    <t>Revisione SD - Svuotare Carrello</t>
+  </si>
+  <si>
+    <t>Aggiunta NavigationalPath</t>
+  </si>
+  <si>
+    <t>Aggiunta Class Diagram</t>
   </si>
 </sst>
 </file>
@@ -511,8 +532,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A7DC815F-E9FE-7F4D-BB4C-8E30E115A67B}" name="Tabella1463" displayName="Tabella1463" ref="B2:E32" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
-  <autoFilter ref="B2:E32" xr:uid="{BFD3B3F1-39AF-574B-B4E2-6DD2F98814AC}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A7DC815F-E9FE-7F4D-BB4C-8E30E115A67B}" name="Tabella1463" displayName="Tabella1463" ref="B2:E38" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
+  <autoFilter ref="B2:E38" xr:uid="{BFD3B3F1-39AF-574B-B4E2-6DD2F98814AC}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -915,10 +936,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF4FF433-BE28-5B49-A7A6-6E0656AE40B0}">
-  <dimension ref="A1:M32"/>
+  <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="85" zoomScaleNormal="168" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView topLeftCell="A8" zoomScaleNormal="168" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1380,6 +1401,80 @@
       <c r="E32" s="12" t="s">
         <v>10</v>
       </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B33" s="2">
+        <v>44881</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B34" s="2">
+        <v>44881</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B35" s="2">
+        <v>44881</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B36" s="10">
+        <v>44881</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B37" s="10">
+        <v>44881</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C38" s="1"/>
+      <c r="E38" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1398,7 +1493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{256147BA-D926-674E-96C3-5C4EE21DE2A0}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
+    <sheetView zoomScale="135" workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -2124,7 +2219,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView zoomScale="135" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:E3"/>
+      <selection activeCell="B4" sqref="B4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2173,9 +2268,18 @@
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="2"/>
-      <c r="C4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="B4" s="2">
+        <v>44880</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="2"/>
@@ -2298,8 +2402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC713557-CF4C-3449-B7F2-607954CE9E41}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView zoomScale="135" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:E3"/>
+    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2348,9 +2452,18 @@
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="2"/>
-      <c r="C4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="B4" s="2">
+        <v>44880</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="2"/>

</xml_diff>